<commit_message>
Presupuesto hecho a espera de correcciones
</commit_message>
<xml_diff>
--- a/presupuesto_proyecto.xlsx
+++ b/presupuesto_proyecto.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianacosta/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianacosta/proyecto_grado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FEDA32E-F47A-0145-ACB3-1198525BF132}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDE7A68-9D9A-4546-80EB-6B4F87AD72B6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CF925E45-4B45-2E44-8FFF-E0C890C8676D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>PRESUPUESTO ANTEPROYECTO</t>
   </si>
@@ -144,9 +144,6 @@
     <t>SUBTOTAL MATERIALES E INSUMOS</t>
   </si>
   <si>
-    <t> $ 3.031.400</t>
-  </si>
-  <si>
     <t>EQUIPOS</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>SUBTOTAL EQUIPOS</t>
   </si>
   <si>
-    <t> $ 3.000.000</t>
-  </si>
-  <si>
     <t>OTROS</t>
   </si>
   <si>
@@ -183,13 +177,7 @@
     <t>SUBTOTAL OTROS</t>
   </si>
   <si>
-    <t> $ 3.200.000</t>
-  </si>
-  <si>
     <t>TOTAL, PRESUPUESTO</t>
-  </si>
-  <si>
-    <t> $ 13’131.400</t>
   </si>
 </sst>
 </file>
@@ -804,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -839,9 +827,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -870,6 +855,162 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -887,9 +1028,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -908,157 +1046,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="9" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1377,11 +1368,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24731BA3-230B-4845-9C45-F35586467522}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
@@ -1390,64 +1385,64 @@
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="76"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="29" t="s">
+      <c r="E5" s="80"/>
+      <c r="F5" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31" t="s">
+      <c r="G5" s="80"/>
+      <c r="H5" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="27" t="s">
+      <c r="I5" s="82"/>
+      <c r="J5" s="78" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1460,9 +1455,9 @@
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="28"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="34"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1477,231 +1472,231 @@
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="36"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="73"/>
       <c r="J7" s="9"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="38" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="42">
+      <c r="D8" s="35"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="29">
         <v>900000</v>
       </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="44">
+      <c r="G8" s="35"/>
+      <c r="H8" s="68">
         <v>900000</v>
       </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="42">
+      <c r="I8" s="69"/>
+      <c r="J8" s="29">
         <v>900000</v>
       </c>
-      <c r="K8" s="48"/>
+      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="48"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="38" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="42">
+      <c r="D10" s="35"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="29">
         <v>6000000</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="44">
+      <c r="G10" s="35"/>
+      <c r="H10" s="68">
         <v>6000000</v>
       </c>
-      <c r="I10" s="45"/>
-      <c r="J10" s="42">
+      <c r="I10" s="69"/>
+      <c r="J10" s="29">
         <v>6000000</v>
       </c>
-      <c r="K10" s="48"/>
+      <c r="K10" s="32"/>
     </row>
     <row r="11" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="48"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="49" t="s">
+      <c r="G12" s="14"/>
+      <c r="H12" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="50"/>
-      <c r="J12" s="15" t="s">
+      <c r="I12" s="47"/>
+      <c r="J12" s="14" t="s">
         <v>25</v>
       </c>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="51"/>
-      <c r="B13" s="53" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="55">
+      <c r="C13" s="52">
         <v>6900000</v>
       </c>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="57"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="54"/>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="60"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="57"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="62"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="70"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="67"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="61"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="70"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="67"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="61"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="70"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="67"/>
     </row>
     <row r="18" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="67"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="70"/>
+      <c r="A18" s="64"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="67"/>
     </row>
     <row r="19" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="71" t="s">
+      <c r="B19" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="73"/>
-      <c r="F19" s="72" t="s">
+      <c r="E19" s="45"/>
+      <c r="F19" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="73"/>
-      <c r="H19" s="71" t="s">
+      <c r="G19" s="45"/>
+      <c r="H19" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="71" t="s">
+      <c r="I19" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="71" t="s">
+      <c r="J19" s="33" t="s">
         <v>7</v>
       </c>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="4" t="s">
         <v>8</v>
       </c>
@@ -1714,13 +1709,13 @@
       <c r="G20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+      <c r="A21" s="15">
         <v>2</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -1736,8 +1731,8 @@
       <c r="J21" s="9"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" ht="34" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+    <row r="22" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="11" t="s">
@@ -1746,78 +1741,86 @@
       <c r="C22" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="17">
         <v>70000</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="18">
-        <v>60000</v>
-      </c>
-      <c r="I22" s="18">
-        <v>71400</v>
-      </c>
-      <c r="J22" s="18">
-        <v>131400</v>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="17">
+        <f>D22+E22+F22+G22</f>
+        <v>70000</v>
+      </c>
+      <c r="I22" s="17">
+        <f>H22-(H22/1.16)</f>
+        <v>9655.1724137931014</v>
+      </c>
+      <c r="J22" s="17">
+        <f>H22-I22</f>
+        <v>60344.827586206899</v>
       </c>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="42">
-        <v>2648700</v>
-      </c>
-      <c r="I23" s="42">
-        <v>51300</v>
-      </c>
-      <c r="J23" s="42">
-        <v>2700000</v>
-      </c>
-      <c r="K23" s="48"/>
+      <c r="D23" s="29">
+        <v>1000000</v>
+      </c>
+      <c r="E23" s="29">
+        <v>200000</v>
+      </c>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="29">
+        <f>D23+E23+F23+G23</f>
+        <v>1200000</v>
+      </c>
+      <c r="I23" s="29">
+        <f>H23-(H23/1.12)</f>
+        <v>128571.42857142864</v>
+      </c>
+      <c r="J23" s="29">
+        <f>H23-I23</f>
+        <v>1071428.5714285714</v>
+      </c>
+      <c r="K23" s="32"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="48"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="18">
-        <v>1000000</v>
-      </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="48"/>
-    </row>
-    <row r="26" spans="1:11" ht="34" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A25" s="37"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="32"/>
+    </row>
+    <row r="26" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -1826,49 +1829,53 @@
       <c r="C26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="17">
         <v>170000</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="18">
-        <v>162000</v>
-      </c>
-      <c r="I26" s="18">
-        <v>38000</v>
-      </c>
-      <c r="J26" s="18">
-        <v>200000</v>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="17">
+        <f>D26+E26+F26+G26</f>
+        <v>170000</v>
+      </c>
+      <c r="I26" s="17">
+        <f>H26-(H26/1.16)</f>
+        <v>23448.275862068956</v>
+      </c>
+      <c r="J26" s="17">
+        <f>H26-I26</f>
+        <v>146551.72413793104</v>
       </c>
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" ht="34" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="21" t="s">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22" t="s">
+      <c r="C27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="85">
+        <f>J21+J22+J23+J26</f>
+        <v>1278325.1231527093</v>
+      </c>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+    </row>
+    <row r="29" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>3</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="79"/>
-    </row>
-    <row r="29" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16">
-        <v>3</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
@@ -1879,57 +1886,61 @@
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="1:11" ht="34" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+    <row r="30" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="C30" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="D30" s="17">
+        <v>7299000</v>
+      </c>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="17">
+        <f>D30+E30+F30+G30</f>
+        <v>7299000</v>
+      </c>
+      <c r="I30" s="17">
+        <f>H30-(H30/1.16)</f>
+        <v>1006758.6206896547</v>
+      </c>
+      <c r="J30" s="17">
+        <f>H30-I30</f>
+        <v>6292241.3793103453</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="B31" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="18">
-        <v>21000000</v>
-      </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="18">
-        <v>1680000</v>
-      </c>
-      <c r="I30" s="18">
-        <v>570000</v>
-      </c>
-      <c r="J30" s="18">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="21" t="s">
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="85">
+        <f>J30</f>
+        <v>6292241.3793103453</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+    </row>
+    <row r="33" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>4</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="79"/>
-    </row>
-    <row r="33" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16">
-        <v>4</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
@@ -1941,88 +1952,139 @@
       <c r="J33" s="9"/>
     </row>
     <row r="34" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="22">
+        <f>50000*4</f>
+        <v>200000</v>
+      </c>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="22">
+        <f>D34+E34+F34+G34</f>
+        <v>200000</v>
+      </c>
+      <c r="I34" s="24"/>
+      <c r="J34" s="17">
+        <f>H34</f>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B35" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="18">
-        <v>2200000</v>
-      </c>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="80"/>
-      <c r="I34" s="80"/>
-      <c r="J34" s="18">
-        <v>2200000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+      <c r="D35" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="22">
+        <f>D35+E35+F35+G35</f>
+        <v>1000000</v>
+      </c>
+      <c r="I35" s="22">
+        <f>H35-(H35/1.16)</f>
+        <v>137931.03448275861</v>
+      </c>
+      <c r="J35" s="25">
+        <f>H35-I35</f>
+        <v>862068.96551724139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="C36" s="20"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="85">
+        <f>J34+J35</f>
+        <v>1062068.9655172415</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+    </row>
+    <row r="38" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="18">
-        <v>1000000</v>
-      </c>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="81">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="21"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="79"/>
-    </row>
-    <row r="38" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="82" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="83"/>
-      <c r="C38" s="83"/>
-      <c r="D38" s="83"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="83"/>
-      <c r="I38" s="84" t="s">
-        <v>54</v>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="86">
+        <f>J27+J31+J36+C13</f>
+        <v>15532635.467980295</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="85"/>
+      <c r="A39" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="53">
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:J14"/>
+    <mergeCell ref="A15:J18"/>
+    <mergeCell ref="K15:K18"/>
     <mergeCell ref="J23:J25"/>
     <mergeCell ref="K23:K25"/>
     <mergeCell ref="I19:I20"/>
@@ -2039,42 +2101,6 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:J14"/>
-    <mergeCell ref="A15:J18"/>
-    <mergeCell ref="K15:K18"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:I9"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I6"/>
-    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Se modifica presupuesto del anteproyecto, y se corrigen errores de redacción y terminación del documento
</commit_message>
<xml_diff>
--- a/presupuesto_proyecto.xlsx
+++ b/presupuesto_proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianacosta/proyecto_grado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDE7A68-9D9A-4546-80EB-6B4F87AD72B6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8582D17B-6383-E047-B62C-8D79EF10A5CD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CF925E45-4B45-2E44-8FFF-E0C890C8676D}"/>
   </bookViews>
@@ -129,9 +129,6 @@
     <t>Software</t>
   </si>
   <si>
-    <t>software de desarrollo, (licencias)</t>
-  </si>
-  <si>
     <t>2.4</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>TOTAL, PRESUPUESTO</t>
+  </si>
+  <si>
+    <t>software de desarrollo, (licencias), Adobe Creative Cloud, externo plantilla web y servidor vps</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -878,6 +878,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="6" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="9" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="6" fontId="8" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -885,48 +891,84 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -995,62 +1037,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="9" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1368,81 +1368,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24731BA3-230B-4845-9C45-F35586467522}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17" thickBot="1">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+    <row r="3" spans="1:11" ht="20" thickBot="1">
+      <c r="A3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="76"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="77"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
+    <row r="4" spans="1:11" ht="17" thickBot="1">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78" t="s">
+    <row r="5" spans="1:11" ht="17" thickBot="1">
+      <c r="A5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="79" t="s">
+      <c r="E5" s="41"/>
+      <c r="F5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="80"/>
-      <c r="H5" s="81" t="s">
+      <c r="G5" s="41"/>
+      <c r="H5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="82"/>
-      <c r="J5" s="78" t="s">
+      <c r="I5" s="43"/>
+      <c r="J5" s="38" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
+    <row r="6" spans="1:11" ht="17" thickBot="1">
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1455,12 +1455,12 @@
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="83"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="34"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="39"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="17" thickBot="1">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -1472,92 +1472,92 @@
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="73"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="9"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+    <row r="8" spans="1:11">
+      <c r="A8" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="50" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="29">
+      <c r="D8" s="48"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="31">
         <v>900000</v>
       </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="68">
+      <c r="G8" s="48"/>
+      <c r="H8" s="52">
         <v>900000</v>
       </c>
-      <c r="I8" s="69"/>
-      <c r="J8" s="29">
+      <c r="I8" s="53"/>
+      <c r="J8" s="31">
         <v>900000</v>
       </c>
-      <c r="K8" s="32"/>
-    </row>
-    <row r="9" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="40"/>
+      <c r="K8" s="56"/>
+    </row>
+    <row r="9" spans="1:11" ht="17" thickBot="1">
+      <c r="A9" s="49"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="D9" s="49"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="56"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="50" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="29">
+      <c r="D10" s="48"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="31">
         <v>6000000</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="68">
+      <c r="G10" s="48"/>
+      <c r="H10" s="52">
         <v>6000000</v>
       </c>
-      <c r="I10" s="69"/>
-      <c r="J10" s="29">
+      <c r="I10" s="53"/>
+      <c r="J10" s="31">
         <v>6000000</v>
       </c>
-      <c r="K10" s="32"/>
-    </row>
-    <row r="11" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="40"/>
+      <c r="K10" s="56"/>
+    </row>
+    <row r="11" spans="1:11" ht="17" thickBot="1">
+      <c r="A11" s="49"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="70"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-    </row>
-    <row r="12" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="49"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="56"/>
+    </row>
+    <row r="12" spans="1:11" ht="17" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
@@ -1573,130 +1573,130 @@
         <v>24</v>
       </c>
       <c r="G12" s="14"/>
-      <c r="H12" s="46" t="s">
+      <c r="H12" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="47"/>
+      <c r="I12" s="61"/>
       <c r="J12" s="14" t="s">
         <v>25</v>
       </c>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="48"/>
-      <c r="B13" s="50" t="s">
+    <row r="13" spans="1:11" ht="17" thickTop="1">
+      <c r="A13" s="62"/>
+      <c r="B13" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="52">
+      <c r="C13" s="66">
         <v>6900000</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="54"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="68"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="57"/>
+    <row r="14" spans="1:11" ht="17" thickBot="1">
+      <c r="A14" s="63"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="71"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="58"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="67"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="61"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="67"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="61"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="67"/>
-    </row>
-    <row r="18" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="64"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="67"/>
-    </row>
-    <row r="19" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+    <row r="15" spans="1:11">
+      <c r="A15" s="72"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="81"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="75"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="77"/>
+      <c r="K16" s="81"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="75"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="77"/>
+      <c r="K17" s="81"/>
+    </row>
+    <row r="18" spans="1:11" ht="17" thickBot="1">
+      <c r="A18" s="78"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="81"/>
+    </row>
+    <row r="19" spans="1:11" ht="17" thickBot="1">
+      <c r="A19" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="44" t="s">
+      <c r="E19" s="58"/>
+      <c r="F19" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="45"/>
-      <c r="H19" s="33" t="s">
+      <c r="G19" s="58"/>
+      <c r="H19" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="I19" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="33" t="s">
+      <c r="J19" s="59" t="s">
         <v>7</v>
       </c>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
+    <row r="20" spans="1:11" ht="17" thickBot="1">
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="4" t="s">
         <v>8</v>
       </c>
@@ -1709,12 +1709,12 @@
       <c r="G20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="23" thickBot="1">
       <c r="A21" s="15">
         <v>2</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="J21" s="9"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="23" thickBot="1">
       <c r="A22" s="16" t="s">
         <v>29</v>
       </c>
@@ -1761,73 +1761,74 @@
       </c>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="35" t="s">
+    <row r="23" spans="1:11">
+      <c r="A23" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="31">
+        <v>759840</v>
+      </c>
+      <c r="E23" s="31">
+        <f>200000+1026000</f>
+        <v>1226000</v>
+      </c>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="31">
+        <f>D23+E23+F23+G23</f>
+        <v>1985840</v>
+      </c>
+      <c r="I23" s="31">
+        <f>H23-(H23/1.12)</f>
+        <v>212768.57142857159</v>
+      </c>
+      <c r="J23" s="31">
+        <f>H23-I23</f>
+        <v>1773071.4285714284</v>
+      </c>
+      <c r="K23" s="56"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="82"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="56"/>
+    </row>
+    <row r="25" spans="1:11" ht="17" thickBot="1">
+      <c r="A25" s="49"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="56"/>
+    </row>
+    <row r="26" spans="1:11" ht="23" thickBot="1">
+      <c r="A26" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="29">
-        <v>1000000</v>
-      </c>
-      <c r="E23" s="29">
-        <v>200000</v>
-      </c>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="29">
-        <f>D23+E23+F23+G23</f>
-        <v>1200000</v>
-      </c>
-      <c r="I23" s="29">
-        <f>H23-(H23/1.12)</f>
-        <v>128571.42857142864</v>
-      </c>
-      <c r="J23" s="29">
-        <f>H23-I23</f>
-        <v>1071428.5714285714</v>
-      </c>
-      <c r="K23" s="32"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="36"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="32"/>
-    </row>
-    <row r="25" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="32"/>
-    </row>
-    <row r="26" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="B26" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>37</v>
       </c>
       <c r="D26" s="17">
         <v>170000</v>
@@ -1849,10 +1850,10 @@
       </c>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" ht="34" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="34" thickBot="1">
       <c r="A27" s="19"/>
       <c r="B27" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
@@ -1861,21 +1862,21 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
-      <c r="J27" s="85">
+      <c r="J27" s="29">
         <f>J21+J22+J23+J26</f>
-        <v>1278325.1231527093</v>
+        <v>1979967.9802955664</v>
       </c>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="17" thickBot="1">
       <c r="A28" s="23"/>
     </row>
-    <row r="29" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="17" thickBot="1">
       <c r="A29" s="15">
         <v>3</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
@@ -1886,15 +1887,15 @@
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="23" thickBot="1">
       <c r="A30" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="C30" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="D30" s="17">
         <v>7299000</v>
@@ -1915,10 +1916,10 @@
         <v>6292241.3793103453</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="23" thickBot="1">
       <c r="A31" s="19"/>
       <c r="B31" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="20"/>
       <c r="D31" s="21"/>
@@ -1927,20 +1928,20 @@
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
       <c r="I31" s="21"/>
-      <c r="J31" s="85">
+      <c r="J31" s="29">
         <f>J30</f>
         <v>6292241.3793103453</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="17" thickBot="1">
       <c r="A32" s="23"/>
     </row>
-    <row r="33" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="17" thickBot="1">
       <c r="A33" s="15">
         <v>4</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
@@ -1951,15 +1952,15 @@
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="17" thickBot="1">
       <c r="A34" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>46</v>
-      </c>
       <c r="C34" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="22">
@@ -1978,15 +1979,15 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="17" thickBot="1">
       <c r="A35" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>48</v>
-      </c>
       <c r="C35" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" s="17">
         <v>1000000</v>
@@ -2007,10 +2008,10 @@
         <v>862068.96551724139</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="17" thickBot="1">
       <c r="A36" s="19"/>
       <c r="B36" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" s="20"/>
       <c r="D36" s="21"/>
@@ -2019,17 +2020,17 @@
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
       <c r="I36" s="21"/>
-      <c r="J36" s="85">
+      <c r="J36" s="29">
         <f>J34+J35</f>
         <v>1062068.9655172415</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="17" thickBot="1">
       <c r="A37" s="23"/>
     </row>
-    <row r="38" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="17" thickBot="1">
       <c r="A38" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B38" s="27"/>
       <c r="C38" s="27"/>
@@ -2038,16 +2039,53 @@
       <c r="F38" s="27"/>
       <c r="G38" s="27"/>
       <c r="H38" s="27"/>
-      <c r="I38" s="86">
+      <c r="I38" s="30">
         <f>J27+J31+J36+C13</f>
-        <v>15532635.467980295</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+        <v>16234278.325123154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="K23:K25"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:J14"/>
+    <mergeCell ref="A15:J18"/>
+    <mergeCell ref="K15:K18"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:I11"/>
+    <mergeCell ref="J10:J11"/>
     <mergeCell ref="D23:D25"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A4:J4"/>
@@ -2064,43 +2102,6 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:J14"/>
-    <mergeCell ref="A15:J18"/>
-    <mergeCell ref="K15:K18"/>
-    <mergeCell ref="J23:J25"/>
-    <mergeCell ref="K23:K25"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>